<commit_message>
changing the province label to uppercase
</commit_message>
<xml_diff>
--- a/x_prediction_3.xlsx
+++ b/x_prediction_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\sherlock-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301FFA3D-0BEE-4576-BFD2-BC79078152A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121B0062-90A2-4786-809C-B5E76EAA2962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,116 +44,116 @@
     <t>x3</t>
   </si>
   <si>
-    <t>Aceh</t>
-  </si>
-  <si>
-    <t>Sumatera Utara</t>
-  </si>
-  <si>
-    <t>Sumatera Barat</t>
-  </si>
-  <si>
-    <t>Riau</t>
-  </si>
-  <si>
-    <t>Jambi</t>
-  </si>
-  <si>
-    <t>Sumatera Selatan</t>
-  </si>
-  <si>
-    <t>Bengkulu</t>
-  </si>
-  <si>
-    <t>Lampung</t>
-  </si>
-  <si>
-    <t>Kepulauan Bangka Belitung</t>
-  </si>
-  <si>
-    <t>Kepulauan Riau</t>
-  </si>
-  <si>
-    <t>DKI Jakarta</t>
-  </si>
-  <si>
-    <t>Jawa Barat</t>
-  </si>
-  <si>
-    <t>Jawa Tengah</t>
-  </si>
-  <si>
-    <t>DI Yogyakarta</t>
-  </si>
-  <si>
-    <t>Jawa Timur</t>
-  </si>
-  <si>
-    <t>Banten</t>
-  </si>
-  <si>
-    <t>Bali</t>
-  </si>
-  <si>
-    <t>Nusa Tenggara Barat</t>
-  </si>
-  <si>
-    <t>Nusa Tenggara Timur</t>
-  </si>
-  <si>
-    <t>Kalimantan Barat</t>
-  </si>
-  <si>
-    <t>Kalimantan Tengah</t>
-  </si>
-  <si>
-    <t>Kalimantan Selatan</t>
-  </si>
-  <si>
-    <t>Kalimantan Timur</t>
-  </si>
-  <si>
-    <t>Kalimantan Utara</t>
-  </si>
-  <si>
-    <t>Sulawesi Utara</t>
-  </si>
-  <si>
-    <t>Sulawesi Tengah</t>
-  </si>
-  <si>
-    <t>Sulawesi Selatan</t>
-  </si>
-  <si>
-    <t>Sulawesi Tenggara</t>
-  </si>
-  <si>
-    <t>Gorontalo</t>
-  </si>
-  <si>
-    <t>Sulawesi Barat</t>
-  </si>
-  <si>
-    <t>Maluku</t>
-  </si>
-  <si>
-    <t>Maluku Utara</t>
-  </si>
-  <si>
-    <t>Papua Barat</t>
-  </si>
-  <si>
-    <t>Papua</t>
-  </si>
-  <si>
     <t>province</t>
+  </si>
+  <si>
+    <t>ACEH</t>
+  </si>
+  <si>
+    <t>SUMATERA UTARA</t>
+  </si>
+  <si>
+    <t>SUMATERA BARAT</t>
+  </si>
+  <si>
+    <t>RIAU</t>
+  </si>
+  <si>
+    <t>JAMBI</t>
+  </si>
+  <si>
+    <t>SUMATERA SELATAN</t>
+  </si>
+  <si>
+    <t>BENGKULU</t>
+  </si>
+  <si>
+    <t>LAMPUNG</t>
+  </si>
+  <si>
+    <t>KEPULAUAN BANGKA BELITUNG</t>
+  </si>
+  <si>
+    <t>KEPULAUAN RIAU</t>
+  </si>
+  <si>
+    <t>DKI JAKARTA</t>
+  </si>
+  <si>
+    <t>JAWA BARAT</t>
+  </si>
+  <si>
+    <t>JAWA TENGAH</t>
+  </si>
+  <si>
+    <t>DAERAH ISTIMEWA YOGYAKARTA</t>
+  </si>
+  <si>
+    <t>JAWA TIMUR</t>
+  </si>
+  <si>
+    <t>BANTEN</t>
+  </si>
+  <si>
+    <t>BALI</t>
+  </si>
+  <si>
+    <t>NUSA TENGGARA BARAT</t>
+  </si>
+  <si>
+    <t>NUSA TENGGARA TIMUR</t>
+  </si>
+  <si>
+    <t>KALIMANTAN BARAT</t>
+  </si>
+  <si>
+    <t>KALIMANTAN TENGAH</t>
+  </si>
+  <si>
+    <t>KALIMANTAN SELATAN</t>
+  </si>
+  <si>
+    <t>KALIMANTAN TIMUR</t>
+  </si>
+  <si>
+    <t>KALIMANTAN UTARA</t>
+  </si>
+  <si>
+    <t>SULAWESI UTARA</t>
+  </si>
+  <si>
+    <t>SULAWESI TENGAH</t>
+  </si>
+  <si>
+    <t>SULAWESI SELATAN</t>
+  </si>
+  <si>
+    <t>SULAWESI TENGGARA</t>
+  </si>
+  <si>
+    <t>GORONTALO</t>
+  </si>
+  <si>
+    <t>SULAWESI BARAT</t>
+  </si>
+  <si>
+    <t>MALUKU</t>
+  </si>
+  <si>
+    <t>MALUKU UTARA</t>
+  </si>
+  <si>
+    <t>PAPUA BARAT</t>
+  </si>
+  <si>
+    <t>PAPUA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,12 +175,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,12 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,13 +525,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="F138" sqref="F138"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -550,9 +545,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
         <v>4.4484243392944336</v>
@@ -564,9 +559,9 @@
         <v>0.30240219831466669</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
         <v>5.1064071655273438</v>
@@ -578,9 +573,9 @@
         <v>0.31409749388694758</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
         <v>4.0730409622192383</v>
@@ -592,9 +587,9 @@
         <v>0.26706832647323608</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
         <v>4.658531665802002</v>
@@ -606,9 +601,9 @@
         <v>0.32878988981246948</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
         <v>3.6874620914459229</v>
@@ -620,9 +615,9 @@
         <v>0.34585019946098328</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
       </c>
       <c r="B7">
         <v>5.0802960395812988</v>
@@ -634,9 +629,9 @@
         <v>0.34076985716819758</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
       <c r="B8">
         <v>4.3285651206970206</v>
@@ -648,9 +643,9 @@
         <v>0.33474111557006841</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
       </c>
       <c r="B9">
         <v>5.2682061195373544</v>
@@ -662,9 +657,9 @@
         <v>0.29739287495613098</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
       </c>
       <c r="B10">
         <v>2.4670875072479248</v>
@@ -676,9 +671,9 @@
         <v>0.2366654425859451</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
       </c>
       <c r="B11">
         <v>5.2722187042236328</v>
@@ -690,9 +685,9 @@
         <v>0.3364633321762085</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
       </c>
       <c r="B12">
         <v>4.0993900299072266</v>
@@ -704,9 +699,9 @@
         <v>0.4240507185459137</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
       </c>
       <c r="B13">
         <v>5.0288963317871094</v>
@@ -718,9 +713,9 @@
         <v>0.40960600972175598</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
       </c>
       <c r="B14">
         <v>5.6789021492004386</v>
@@ -732,9 +727,9 @@
         <v>0.37532514333724981</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
       </c>
       <c r="B15">
         <v>5.0865931510925293</v>
@@ -746,9 +741,9 @@
         <v>0.4240507185459137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
       </c>
       <c r="B16">
         <v>5.2561616897583008</v>
@@ -760,9 +755,9 @@
         <v>0.37810149788856512</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
       </c>
       <c r="B17">
         <v>5.8734455108642578</v>
@@ -774,9 +769,9 @@
         <v>0.37373071908950811</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
       </c>
       <c r="B18">
         <v>6.0203714370727539</v>
@@ -788,9 +783,9 @@
         <v>0.3663966953754425</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
       </c>
       <c r="B19">
         <v>4.2437467575073242</v>
@@ -802,9 +797,9 @@
         <v>0.37351292371749878</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <v>4.337158203125</v>
@@ -816,9 +811,9 @@
         <v>0.33030503988265991</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
       </c>
       <c r="B21">
         <v>5.2311630249023438</v>
@@ -830,9 +825,9 @@
         <v>0.31157100200653082</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
       </c>
       <c r="B22">
         <v>5.842191219329834</v>
@@ -844,9 +839,9 @@
         <v>0.32574373483657842</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
       </c>
       <c r="B23">
         <v>6.0802693367004386</v>
@@ -858,9 +853,9 @@
         <v>0.31564828753471369</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
       </c>
       <c r="B24">
         <v>5.7494850158691406</v>
@@ -872,9 +867,9 @@
         <v>0.32702603936195368</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>26</v>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
       </c>
       <c r="B25">
         <v>6.6852970123291016</v>
@@ -886,9 +881,9 @@
         <v>0.27474889159202581</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>27</v>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
       </c>
       <c r="B26">
         <v>4.3266777992248544</v>
@@ -900,9 +895,9 @@
         <v>0.36376684904098511</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>28</v>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
       </c>
       <c r="B27">
         <v>10.83905506134033</v>
@@ -914,9 +909,9 @@
         <v>0.29723566770553589</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
       </c>
       <c r="B28">
         <v>4.7645688056945801</v>
@@ -928,9 +923,9 @@
         <v>0.36936596035957342</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>30</v>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
       </c>
       <c r="B29">
         <v>5.129481315612793</v>
@@ -942,9 +937,9 @@
         <v>0.37469109892845148</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>31</v>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
       </c>
       <c r="B30">
         <v>5.2427096366882324</v>
@@ -956,9 +951,9 @@
         <v>0.41637623310089111</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>32</v>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
       </c>
       <c r="B31">
         <v>5.8045368194580078</v>
@@ -970,9 +965,9 @@
         <v>0.35774749517440801</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>33</v>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>34</v>
       </c>
       <c r="B32">
         <v>4.9164152145385742</v>
@@ -984,9 +979,9 @@
         <v>0.28722968697547913</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>34</v>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>35</v>
       </c>
       <c r="B33">
         <v>16.029935836791989</v>
@@ -998,9 +993,9 @@
         <v>0.31009644269943237</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>35</v>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>36</v>
       </c>
       <c r="B34">
         <v>5.8254303932189941</v>
@@ -1012,9 +1007,9 @@
         <v>0.3708406388759613</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>36</v>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>37</v>
       </c>
       <c r="B35">
         <v>8.6052999496459961</v>
@@ -1026,9 +1021,9 @@
         <v>0.39537414908409119</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>3</v>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>4</v>
       </c>
       <c r="B36">
         <v>4.3891339302062988</v>
@@ -1040,9 +1035,9 @@
         <v>0.3065263032913208</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>4</v>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5</v>
       </c>
       <c r="B37">
         <v>5.6552615165710449</v>
@@ -1054,9 +1049,9 @@
         <v>0.31076076626777649</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>5</v>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>6</v>
       </c>
       <c r="B38">
         <v>4.2018857002258301</v>
@@ -1068,9 +1063,9 @@
         <v>0.26495450735092158</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>7</v>
       </c>
       <c r="B39">
         <v>5.1282124519348136</v>
@@ -1082,9 +1077,9 @@
         <v>0.33108067512512213</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>7</v>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>8</v>
       </c>
       <c r="B40">
         <v>3.6538040637969971</v>
@@ -1096,9 +1091,9 @@
         <v>0.34087401628494263</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>8</v>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>9</v>
       </c>
       <c r="B41">
         <v>4.9355425834655762</v>
@@ -1110,9 +1105,9 @@
         <v>0.344186931848526</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>9</v>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>10</v>
       </c>
       <c r="B42">
         <v>4.4987912178039551</v>
@@ -1124,9 +1119,9 @@
         <v>0.33597475290298462</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>10</v>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>11</v>
       </c>
       <c r="B43">
         <v>5.6234745979309082</v>
@@ -1138,9 +1133,9 @@
         <v>0.2932661771774292</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>11</v>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>12</v>
       </c>
       <c r="B44">
         <v>2.3015353679656978</v>
@@ -1152,9 +1147,9 @@
         <v>0.236572340130806</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>12</v>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>13</v>
       </c>
       <c r="B45">
         <v>5.5831851959228516</v>
@@ -1166,9 +1161,9 @@
         <v>0.33757287263870239</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>13</v>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>14</v>
       </c>
       <c r="B46">
         <v>4.245152473449707</v>
@@ -1180,9 +1175,9 @@
         <v>0.4240507185459137</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>14</v>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>15</v>
       </c>
       <c r="B47">
         <v>5.1322236061096191</v>
@@ -1194,9 +1189,9 @@
         <v>0.41003111004829412</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>15</v>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>16</v>
       </c>
       <c r="B48">
         <v>6.1120662689208984</v>
@@ -1208,9 +1203,9 @@
         <v>0.38126683235168463</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>16</v>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>17</v>
       </c>
       <c r="B49">
         <v>5.6605992317199707</v>
@@ -1222,9 +1217,9 @@
         <v>0.42345735430717468</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>17</v>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>18</v>
       </c>
       <c r="B50">
         <v>5.5807414054870614</v>
@@ -1236,9 +1231,9 @@
         <v>0.37345421314239502</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>18</v>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>19</v>
       </c>
       <c r="B51">
         <v>6.707770824432373</v>
@@ -1250,9 +1245,9 @@
         <v>0.37690433859825129</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>19</v>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>20</v>
       </c>
       <c r="B52">
         <v>6.1550850868225098</v>
@@ -1264,9 +1259,9 @@
         <v>0.37068188190460211</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>20</v>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>21</v>
       </c>
       <c r="B53">
         <v>5.6300482749938956</v>
@@ -1278,9 +1273,9 @@
         <v>0.37336564064025879</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>21</v>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>22</v>
       </c>
       <c r="B54">
         <v>5.3392739295959473</v>
@@ -1292,9 +1287,9 @@
         <v>0.33381718397140497</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>22</v>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>23</v>
       </c>
       <c r="B55">
         <v>5.7497310638427734</v>
@@ -1306,9 +1301,9 @@
         <v>0.30364620685577393</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>23</v>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>24</v>
       </c>
       <c r="B56">
         <v>6.2213907241821289</v>
@@ -1320,9 +1315,9 @@
         <v>0.3219236433506012</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>24</v>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>25</v>
       </c>
       <c r="B57">
         <v>6.4782505035400391</v>
@@ -1334,9 +1329,9 @@
         <v>0.31978479027748108</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>25</v>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>26</v>
       </c>
       <c r="B58">
         <v>5.9729251861572266</v>
@@ -1348,9 +1343,9 @@
         <v>0.32771152257919312</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>26</v>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>27</v>
       </c>
       <c r="B59">
         <v>7.4800200462341309</v>
@@ -1362,9 +1357,9 @@
         <v>0.2726554274559021</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>27</v>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>28</v>
       </c>
       <c r="B60">
         <v>4.4063472747802734</v>
@@ -1376,9 +1371,9 @@
         <v>0.35967722535133362</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>28</v>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>29</v>
       </c>
       <c r="B61">
         <v>9.9127941131591797</v>
@@ -1390,9 +1385,9 @@
         <v>0.30116966366767878</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>29</v>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>30</v>
       </c>
       <c r="B62">
         <v>5.1669731140136719</v>
@@ -1404,9 +1399,9 @@
         <v>0.36644446849822998</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>30</v>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>31</v>
       </c>
       <c r="B63">
         <v>5.2308268547058114</v>
@@ -1418,9 +1413,9 @@
         <v>0.3781430721282959</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>31</v>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>32</v>
       </c>
       <c r="B64">
         <v>5.2904624938964844</v>
@@ -1432,9 +1427,9 @@
         <v>0.41940462589263922</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>32</v>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>33</v>
       </c>
       <c r="B65">
         <v>5.7300033569335938</v>
@@ -1446,9 +1441,9 @@
         <v>0.35541573166847229</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>33</v>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>34</v>
       </c>
       <c r="B66">
         <v>5.3704285621643066</v>
@@ -1460,9 +1455,9 @@
         <v>0.29068249464035029</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>34</v>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>35</v>
       </c>
       <c r="B67">
         <v>12.951755523681641</v>
@@ -1474,9 +1469,9 @@
         <v>0.30965286493301392</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>35</v>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>36</v>
       </c>
       <c r="B68">
         <v>6.3608207702636719</v>
@@ -1488,9 +1483,9 @@
         <v>0.37048643827438349</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>36</v>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>37</v>
       </c>
       <c r="B69">
         <v>7.9650082588195801</v>
@@ -1502,9 +1497,9 @@
         <v>0.39667344093322748</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>3</v>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>4</v>
       </c>
       <c r="B70">
         <v>4.2506523132324219</v>
@@ -1516,9 +1511,9 @@
         <v>0.30950447916984558</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>4</v>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>5</v>
       </c>
       <c r="B71">
         <v>5.8436369895935059</v>
@@ -1530,9 +1525,9 @@
         <v>0.30683025717735291</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>5</v>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>6</v>
       </c>
       <c r="B72">
         <v>4.0465307235717773</v>
@@ -1544,9 +1539,9 @@
         <v>0.2647155225276947</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>6</v>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>7</v>
       </c>
       <c r="B73">
         <v>5.2707118988037109</v>
@@ -1558,9 +1553,9 @@
         <v>0.330771803855896</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>7</v>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>8</v>
       </c>
       <c r="B74">
         <v>3.8848779201507568</v>
@@ -1572,9 +1567,9 @@
         <v>0.33701783418655401</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>8</v>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>9</v>
       </c>
       <c r="B75">
         <v>4.8399930000305176</v>
@@ -1586,9 +1581,9 @@
         <v>0.34800627827644348</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>9</v>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>10</v>
       </c>
       <c r="B76">
         <v>4.6544842720031738</v>
@@ -1600,9 +1595,9 @@
         <v>0.33632099628448492</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>10</v>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>11</v>
       </c>
       <c r="B77">
         <v>5.9205594062805176</v>
@@ -1614,9 +1609,9 @@
         <v>0.28952726721763611</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>11</v>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>12</v>
       </c>
       <c r="B78">
         <v>2.9800572395324711</v>
@@ -1628,9 +1623,9 @@
         <v>0.2358774542808533</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>12</v>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>13</v>
       </c>
       <c r="B79">
         <v>5.8297381401062012</v>
@@ -1642,9 +1637,9 @@
         <v>0.33931228518486017</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>13</v>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>14</v>
       </c>
       <c r="B80">
         <v>4.5517725944519043</v>
@@ -1656,9 +1651,9 @@
         <v>0.4240507185459137</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>14</v>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>15</v>
       </c>
       <c r="B81">
         <v>5.2590503692626953</v>
@@ -1670,9 +1665,9 @@
         <v>0.41186180710792542</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>15</v>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>16</v>
       </c>
       <c r="B82">
         <v>6.4267745018005371</v>
@@ -1684,9 +1679,9 @@
         <v>0.38671761751174932</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
-        <v>16</v>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>17</v>
       </c>
       <c r="B83">
         <v>6.1381955146789551</v>
@@ -1698,9 +1693,9 @@
         <v>0.4213249683380127</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
-        <v>17</v>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>18</v>
       </c>
       <c r="B84">
         <v>5.6642379760742188</v>
@@ -1712,9 +1707,9 @@
         <v>0.37107518315315252</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>18</v>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>19</v>
       </c>
       <c r="B85">
         <v>7.2940564155578613</v>
@@ -1726,9 +1721,9 @@
         <v>0.37879973649978638</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>19</v>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>20</v>
       </c>
       <c r="B86">
         <v>6.2461085319519043</v>
@@ -1740,9 +1735,9 @@
         <v>0.374471515417099</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>20</v>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>21</v>
       </c>
       <c r="B87">
         <v>6.6158442497253418</v>
@@ -1754,9 +1749,9 @@
         <v>0.37446904182434082</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>21</v>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>22</v>
       </c>
       <c r="B88">
         <v>5.8782291412353516</v>
@@ -1768,9 +1763,9 @@
         <v>0.33610719442367548</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>22</v>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>23</v>
       </c>
       <c r="B89">
         <v>6.0913052558898926</v>
@@ -1782,9 +1777,9 @@
         <v>0.2961181104183197</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>23</v>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>24</v>
       </c>
       <c r="B90">
         <v>6.3162884712219238</v>
@@ -1796,9 +1791,9 @@
         <v>0.31788724660873408</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>24</v>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>25</v>
       </c>
       <c r="B91">
         <v>6.5207839012145996</v>
@@ -1810,9 +1805,9 @@
         <v>0.32396703958511353</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>25</v>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>26</v>
       </c>
       <c r="B92">
         <v>6.0858774185180664</v>
@@ -1824,9 +1819,9 @@
         <v>0.32761463522911072</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>26</v>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>27</v>
       </c>
       <c r="B93">
         <v>7.5715212821960449</v>
@@ -1838,9 +1833,9 @@
         <v>0.27109542489051819</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
-        <v>27</v>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>28</v>
       </c>
       <c r="B94">
         <v>4.6388134956359863</v>
@@ -1852,9 +1847,9 @@
         <v>0.35640540719032288</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>28</v>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>29</v>
       </c>
       <c r="B95">
         <v>8.9662008285522461</v>
@@ -1866,9 +1861,9 @@
         <v>0.3030586838722229</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>29</v>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>30</v>
       </c>
       <c r="B96">
         <v>5.1947822570800781</v>
@@ -1880,9 +1875,9 @@
         <v>0.36461487412452698</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
-        <v>30</v>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>31</v>
       </c>
       <c r="B97">
         <v>5.3219742774963379</v>
@@ -1894,9 +1889,9 @@
         <v>0.38171574473381042</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
-        <v>31</v>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>32</v>
       </c>
       <c r="B98">
         <v>5.0974521636962891</v>
@@ -1908,9 +1903,9 @@
         <v>0.42162248492240911</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
-        <v>32</v>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>33</v>
       </c>
       <c r="B99">
         <v>5.5870270729064941</v>
@@ -1922,9 +1917,9 @@
         <v>0.35421416163444519</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
-        <v>33</v>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>34</v>
       </c>
       <c r="B100">
         <v>5.4949765205383301</v>
@@ -1936,9 +1931,9 @@
         <v>0.2935355007648468</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
-        <v>34</v>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>35</v>
       </c>
       <c r="B101">
         <v>10.72490882873535</v>
@@ -1950,9 +1945,9 @@
         <v>0.3088211715221405</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
-        <v>35</v>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>36</v>
       </c>
       <c r="B102">
         <v>6.4556436538696289</v>
@@ -1964,9 +1959,9 @@
         <v>0.37013432383537292</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>36</v>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>37</v>
       </c>
       <c r="B103">
         <v>7.5124616622924796</v>
@@ -1978,9 +1973,9 @@
         <v>0.39883464574813843</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
-        <v>3</v>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>4</v>
       </c>
       <c r="B104">
         <v>4.2484736442565918</v>
@@ -1992,9 +1987,9 @@
         <v>0.31147980690002441</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>4</v>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>5</v>
       </c>
       <c r="B105">
         <v>5.8928189277648926</v>
@@ -2006,9 +2001,9 @@
         <v>0.3030681312084198</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>5</v>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>6</v>
       </c>
       <c r="B106">
         <v>4.1157889366149902</v>
@@ -2020,9 +2015,9 @@
         <v>0.26516011357307429</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>6</v>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>7</v>
       </c>
       <c r="B107">
         <v>5.3292179107666016</v>
@@ -2034,9 +2029,9 @@
         <v>0.32887184619903559</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>7</v>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>8</v>
       </c>
       <c r="B108">
         <v>4.2387814521789551</v>
@@ -2048,9 +2043,9 @@
         <v>0.33388599753379822</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
-        <v>8</v>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>9</v>
       </c>
       <c r="B109">
         <v>4.9049444198608398</v>
@@ -2062,9 +2057,9 @@
         <v>0.3521895706653595</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>9</v>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>10</v>
       </c>
       <c r="B110">
         <v>4.832639217376709</v>
@@ -2076,9 +2071,9 @@
         <v>0.33597275614738459</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
-        <v>10</v>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>11</v>
       </c>
       <c r="B111">
         <v>6.2086353302001953</v>
@@ -2090,9 +2085,9 @@
         <v>0.28595438599586492</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>11</v>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>12</v>
       </c>
       <c r="B112">
         <v>3.6913378238677979</v>
@@ -2104,9 +2099,9 @@
         <v>0.2351201921701431</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
-        <v>12</v>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>13</v>
       </c>
       <c r="B113">
         <v>6.0908102989196777</v>
@@ -2118,9 +2113,9 @@
         <v>0.34085366129875178</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
-        <v>13</v>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>14</v>
       </c>
       <c r="B114">
         <v>4.8973350524902344</v>
@@ -2132,9 +2127,9 @@
         <v>0.4240507185459137</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
-        <v>14</v>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>15</v>
       </c>
       <c r="B115">
         <v>5.436366081237793</v>
@@ -2146,9 +2141,9 @@
         <v>0.41472789645195007</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
-        <v>15</v>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>16</v>
       </c>
       <c r="B116">
         <v>6.6202764511108398</v>
@@ -2160,9 +2155,9 @@
         <v>0.39134114980697632</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>16</v>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>17</v>
       </c>
       <c r="B117">
         <v>6.4582948684692383</v>
@@ -2174,9 +2169,9 @@
         <v>0.41863632202148438</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>17</v>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>18</v>
       </c>
       <c r="B118">
         <v>5.7981867790222168</v>
@@ -2188,9 +2183,9 @@
         <v>0.37002724409103388</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
-        <v>18</v>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>19</v>
       </c>
       <c r="B119">
         <v>7.5080709457397461</v>
@@ -2202,9 +2197,9 @@
         <v>0.37984970211982733</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>19</v>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>20</v>
       </c>
       <c r="B120">
         <v>6.308072566986084</v>
@@ -2216,9 +2211,9 @@
         <v>0.37791374325752258</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>20</v>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>21</v>
       </c>
       <c r="B121">
         <v>7.1301798820495614</v>
@@ -2230,9 +2225,9 @@
         <v>0.37660583853721619</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
-        <v>21</v>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>22</v>
       </c>
       <c r="B122">
         <v>6.1196584701538086</v>
@@ -2244,9 +2239,9 @@
         <v>0.3373945951461792</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
-        <v>22</v>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>23</v>
       </c>
       <c r="B123">
         <v>6.2878546714782706</v>
@@ -2258,9 +2253,9 @@
         <v>0.28871569037437439</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
-        <v>23</v>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>24</v>
       </c>
       <c r="B124">
         <v>6.2356562614440918</v>
@@ -2272,9 +2267,9 @@
         <v>0.3141472339630127</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
-        <v>24</v>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>25</v>
       </c>
       <c r="B125">
         <v>6.3902087211608887</v>
@@ -2286,9 +2281,9 @@
         <v>0.3275943398475647</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
-        <v>25</v>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>26</v>
       </c>
       <c r="B126">
         <v>6.087618350982666</v>
@@ -2300,9 +2295,9 @@
         <v>0.32721000909805298</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
-        <v>26</v>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>27</v>
       </c>
       <c r="B127">
         <v>7.3504843711853027</v>
@@ -2314,9 +2309,9 @@
         <v>0.2701924741268158</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
-        <v>27</v>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>28</v>
       </c>
       <c r="B128">
         <v>4.9561724662780762</v>
@@ -2328,9 +2323,9 @@
         <v>0.35329899191856379</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
-        <v>28</v>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>29</v>
       </c>
       <c r="B129">
         <v>8.1481647491455078</v>
@@ -2342,9 +2337,9 @@
         <v>0.30370116233825678</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
-        <v>29</v>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>30</v>
       </c>
       <c r="B130">
         <v>5.0793976783752441</v>
@@ -2356,9 +2351,9 @@
         <v>0.36351519823074341</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
-        <v>30</v>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>31</v>
       </c>
       <c r="B131">
         <v>5.3793454170227051</v>
@@ -2370,9 +2365,9 @@
         <v>0.38533881306648249</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>31</v>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>32</v>
       </c>
       <c r="B132">
         <v>4.9037313461303711</v>
@@ -2384,9 +2379,9 @@
         <v>0.42332801222801208</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="2" t="s">
-        <v>32</v>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>33</v>
       </c>
       <c r="B133">
         <v>5.4401249885559082</v>
@@ -2398,9 +2393,9 @@
         <v>0.3540152907371521</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
-        <v>33</v>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>34</v>
       </c>
       <c r="B134">
         <v>5.5066895484924316</v>
@@ -2412,9 +2407,9 @@
         <v>0.29585090279579163</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
-        <v>34</v>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>35</v>
       </c>
       <c r="B135">
         <v>9.1578502655029297</v>
@@ -2426,9 +2421,9 @@
         <v>0.30743375420570368</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
-        <v>35</v>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>36</v>
       </c>
       <c r="B136">
         <v>6.3872995376586914</v>
@@ -2440,9 +2435,9 @@
         <v>0.37026104331016541</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>36</v>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>37</v>
       </c>
       <c r="B137">
         <v>7.2104883193969727</v>

</xml_diff>